<commit_message>
ekim ayı verisi güncellemesi
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurokur\Desktop\kişisel bilgilerim\python_uygulama\temp\myInfilationAPIs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurokur\Desktop\kişisel bilgilerim\python_uygulama\python_backends\turkey_infilation_table\published_ver\myInfilationAPIs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -719,7 +719,7 @@
   <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2197,7 +2197,9 @@
       <c r="I36" s="4">
         <v>80.209999999999994</v>
       </c>
-      <c r="J36" s="4"/>
+      <c r="J36" s="4">
+        <v>85.51</v>
+      </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
@@ -2230,7 +2232,9 @@
       <c r="I37" s="4">
         <v>1.46</v>
       </c>
-      <c r="J37" s="4"/>
+      <c r="J37" s="4">
+        <v>3.54</v>
+      </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>

</xml_diff>